<commit_message>
Functioning realstic instance R2
</commit_message>
<xml_diff>
--- a/instances/description.xlsx
+++ b/instances/description.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\wm-stochastic\instances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\STECCAGIUSEPPE\git\wm-stochastic\instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E8135A-F1B9-4F14-993B-F3B00493108A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1790F0-F728-4818-8263-A21EFEE369BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6135" yWindow="1695" windowWidth="21600" windowHeight="11385" xr2:uid="{B8E7D403-B7B9-4B1A-BBDE-FF9EDC133697}"/>
+    <workbookView xWindow="2820" yWindow="1524" windowWidth="17280" windowHeight="9960" xr2:uid="{B8E7D403-B7B9-4B1A-BBDE-FF9EDC133697}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>I1_S1</t>
   </si>
@@ -78,6 +78,18 @@
   </si>
   <si>
     <t>rispetto alla precedente penalità 5</t>
+  </si>
+  <si>
+    <t>I1_R1</t>
+  </si>
+  <si>
+    <t>I1_R2</t>
+  </si>
+  <si>
+    <t>Reale (penalità 5)</t>
+  </si>
+  <si>
+    <t>Reale (penalità 20) + capacità 1000 + service time 120</t>
   </si>
 </sst>
 </file>
@@ -113,8 +125,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -449,15 +462,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5879FB5A-3DED-49B7-B8D0-3A1A743377ED}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -465,17 +478,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -483,7 +496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -491,7 +504,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -499,7 +512,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -507,13 +520,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>